<commit_message>
Fixes and cleaned up treatment definitions.
Committing files before I switch branches to debug why the questions aren't loading.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FC9060-B289-A948-A0A8-84F340C105BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F418B5A-71E9-9A4E-87D3-AB5879B5ECFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Screen Size Zooming" sheetId="5" r:id="rId3"/>
     <sheet name="Worker Rate" sheetId="7" r:id="rId4"/>
     <sheet name="Holden et al." sheetId="4" r:id="rId5"/>
-    <sheet name="Web Parameters" sheetId="1" r:id="rId6"/>
+    <sheet name="Web Parameters" sheetId="8" r:id="rId6"/>
+    <sheet name="Web Parameters v1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="122">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -428,6 +429,12 @@
   </si>
   <si>
     <t>earlierAmount</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>Read 2001 example, absolute size</t>
   </si>
 </sst>
 </file>
@@ -676,6 +683,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,15 +729,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -726,15 +742,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1079,105 +1086,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1196,7 +1203,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1224,16 +1231,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1734,11 +1741,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1754,6 +1756,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2912,12 +2919,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86262417-1283-894E-BFF0-F5DD2E135B8D}">
-  <dimension ref="A1:U40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3008,6 +3015,344 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>1000</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>1000</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
+        <v>480</v>
+      </c>
+      <c r="N2">
+        <v>480</v>
+      </c>
+      <c r="O2">
+        <v>0.5</v>
+      </c>
+      <c r="P2">
+        <v>0.5</v>
+      </c>
+      <c r="Q2">
+        <v>6</v>
+      </c>
+      <c r="R2">
+        <v>6</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ref="S2" si="0">Q2+O2</f>
+        <v>6.5</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ref="T2" si="1">R2+P2</f>
+        <v>6.5</v>
+      </c>
+      <c r="U2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3">
+        <v>500</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1000</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>1000</v>
+      </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>480</v>
+      </c>
+      <c r="N3">
+        <v>480</v>
+      </c>
+      <c r="O3">
+        <v>0.5</v>
+      </c>
+      <c r="P3">
+        <v>0.5</v>
+      </c>
+      <c r="Q3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <v>6</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3" si="2">Q3+O3</f>
+        <v>6.5</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3" si="3">R3+P3</f>
+        <v>6.5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>480</v>
+      </c>
+      <c r="N4">
+        <v>480</v>
+      </c>
+      <c r="O4">
+        <v>0.5</v>
+      </c>
+      <c r="P4">
+        <v>0.5</v>
+      </c>
+      <c r="Q4">
+        <v>6</v>
+      </c>
+      <c r="R4">
+        <v>6</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ref="S4" si="4">Q4+O4</f>
+        <v>6.5</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4" si="5">R4+P4</f>
+        <v>6.5</v>
+      </c>
+      <c r="U4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5">
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>1000</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>480</v>
+      </c>
+      <c r="N5">
+        <v>480</v>
+      </c>
+      <c r="O5">
+        <v>0.5</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ref="S5:T5" si="6">Q5+O5</f>
+        <v>6.5</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>6.5</v>
+      </c>
+      <c r="U5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86262417-1283-894E-BFF0-F5DD2E135B8D}">
+  <dimension ref="A1:U40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" customWidth="1"/>
+    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="14" max="14" width="24.5" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" customWidth="1"/>
+    <col min="20" max="20" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>104</v>
       </c>
       <c r="D2" t="s">

</xml_diff>

<commit_message>
Changed barchart to show latest answer data.
Fixed the barchart so that it shows the latest answer data.  Also fixed bugs including not loading the new variable_amount parameter from csv, bug in calcTitrationAmount and not capturing the choice time.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD1588C-148C-3845-90D0-A1A3491F90C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1839213-F2B2-B648-9D86-48E938E63189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="6" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -440,10 +440,10 @@
     <t>interaction</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
     <t>variable_amount</t>
+  </si>
+  <si>
+    <t>laterAmount</t>
   </si>
 </sst>
 </file>
@@ -692,6 +692,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,15 +738,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,15 +751,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,105 +1095,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1240,16 +1240,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1750,11 +1750,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1770,6 +1765,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2931,9 +2931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D5"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3047,37 +3047,8 @@
       <c r="J2">
         <v>3</v>
       </c>
-      <c r="L2">
-        <v>1000</v>
-      </c>
       <c r="M2">
         <v>10</v>
-      </c>
-      <c r="N2">
-        <v>480</v>
-      </c>
-      <c r="O2">
-        <v>480</v>
-      </c>
-      <c r="P2">
-        <v>0.5</v>
-      </c>
-      <c r="Q2">
-        <v>0.5</v>
-      </c>
-      <c r="R2">
-        <v>6</v>
-      </c>
-      <c r="S2">
-        <v>6</v>
-      </c>
-      <c r="T2">
-        <f t="shared" ref="T2" si="0">R2+P2</f>
-        <v>6.5</v>
-      </c>
-      <c r="U2">
-        <f t="shared" ref="U2" si="1">S2+Q2</f>
-        <v>6.5</v>
       </c>
       <c r="V2" t="s">
         <v>121</v>
@@ -3136,11 +3107,11 @@
         <v>6</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3" si="2">R3+P3</f>
+        <f t="shared" ref="T3" si="0">R3+P3</f>
         <v>6.5</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3" si="3">S3+Q3</f>
+        <f t="shared" ref="U3" si="1">S3+Q3</f>
         <v>6.5</v>
       </c>
       <c r="V3" t="s">
@@ -3161,7 +3132,7 @@
         <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F4">
         <v>500</v>
@@ -3175,37 +3146,8 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="L4">
-        <v>1000</v>
-      </c>
       <c r="M4">
         <v>10</v>
-      </c>
-      <c r="N4">
-        <v>480</v>
-      </c>
-      <c r="O4">
-        <v>480</v>
-      </c>
-      <c r="P4">
-        <v>0.5</v>
-      </c>
-      <c r="Q4">
-        <v>0.5</v>
-      </c>
-      <c r="R4">
-        <v>6</v>
-      </c>
-      <c r="S4">
-        <v>6</v>
-      </c>
-      <c r="T4">
-        <f t="shared" ref="T4" si="4">R4+P4</f>
-        <v>6.5</v>
-      </c>
-      <c r="U4">
-        <f t="shared" ref="U4" si="5">S4+Q4</f>
-        <v>6.5</v>
       </c>
       <c r="V4" t="s">
         <v>121</v>
@@ -3225,7 +3167,7 @@
         <v>117</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F5">
         <v>500</v>
@@ -3240,7 +3182,7 @@
         <v>10</v>
       </c>
       <c r="L5">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="M5">
         <v>10</v>
@@ -3264,11 +3206,11 @@
         <v>6</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:U5" si="6">R5+P5</f>
+        <f t="shared" ref="T5:U5" si="2">R5+P5</f>
         <v>6.5</v>
       </c>
       <c r="U5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
       <c r="V5" t="s">
@@ -3284,7 +3226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86262417-1283-894E-BFF0-F5DD2E135B8D}">
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
@@ -3319,7 +3261,7 @@
         <v>122</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
Started adding graph treatment to spreadsheet.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1839213-F2B2-B648-9D86-48E938E63189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1A382-71A9-824F-8C18-84B0DDB1F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -692,24 +692,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -738,6 +720,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -751,6 +742,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,105 +1095,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="39" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="49"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="55" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="S3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="50"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1240,16 +1240,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="54"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1750,6 +1750,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1765,11 +1770,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2929,11 +2929,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3217,6 +3217,26 @@
         <v>121</v>
       </c>
     </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3228,7 +3248,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Added logic for bar drag and click to work correctly.
Added logic to make bar click and drag work for the appropriate interaction from the treatment config.
Fixed bugs with divs inside p tag, deleted unused file GistDesign.js, bug with interaction not getting set in Answer.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D1A382-71A9-824F-8C18-84B0DDB1F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6165E4B5-9643-6C46-90A9-81C768D9093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="125">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -692,6 +692,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -720,15 +738,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,15 +751,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,105 +1095,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1240,16 +1240,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1750,11 +1750,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1770,6 +1765,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2929,11 +2929,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3126,13 +3126,13 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F4">
         <v>500</v>
@@ -3146,8 +3146,11 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="M4">
-        <v>10</v>
+      <c r="T4">
+        <v>6</v>
+      </c>
+      <c r="U4">
+        <v>6</v>
       </c>
       <c r="V4" t="s">
         <v>121</v>
@@ -3155,13 +3158,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D5" t="s">
         <v>117</v>
@@ -3179,61 +3182,116 @@
         <v>1000</v>
       </c>
       <c r="J5">
-        <v>10</v>
-      </c>
-      <c r="L5">
-        <v>2000</v>
+        <v>3</v>
       </c>
       <c r="M5">
         <v>10</v>
       </c>
-      <c r="N5">
+      <c r="V5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="L6">
+        <v>2000</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
         <v>480</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>480</v>
       </c>
-      <c r="P5">
+      <c r="P6">
         <v>0.5</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
         <v>0.5</v>
       </c>
-      <c r="R5">
+      <c r="R6">
         <v>6</v>
       </c>
-      <c r="S5">
+      <c r="S6">
         <v>6</v>
       </c>
-      <c r="T5">
-        <f t="shared" ref="T5:U5" si="2">R5+P5</f>
+      <c r="T6">
+        <f t="shared" ref="T6:U6" si="2">R6+P6</f>
         <v>6.5</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6">
+    <row r="7" spans="1:22">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>113</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>118</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F6">
+      <c r="F7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F8">
         <v>500</v>
       </c>
     </row>
@@ -3248,7 +3306,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Fixed bugs and added more treatments to the file.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6165E4B5-9643-6C46-90A9-81C768D9093C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03951AE6-2D00-6C46-BDB2-1B7DA70AFAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="126">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>laterAmount</t>
+  </si>
+  <si>
+    <t>drag</t>
   </si>
 </sst>
 </file>
@@ -692,24 +695,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -738,6 +723,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -751,6 +745,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1095,105 +1098,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="39" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="49"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="55" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="S3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="50"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1215,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1240,16 +1243,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="54"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1750,6 +1753,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1765,11 +1773,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2929,11 +2932,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3045,7 +3048,7 @@
         <v>1000</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M2">
         <v>10</v>
@@ -3056,13 +3059,13 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>118</v>
@@ -3071,62 +3074,33 @@
         <v>118</v>
       </c>
       <c r="F3">
-        <v>500</v>
+        <v>50</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="J3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>1000</v>
+        <v>7</v>
       </c>
       <c r="M3">
         <v>10</v>
       </c>
-      <c r="N3">
-        <v>480</v>
-      </c>
-      <c r="O3">
-        <v>480</v>
-      </c>
-      <c r="P3">
-        <v>0.5</v>
-      </c>
-      <c r="Q3">
-        <v>0.5</v>
-      </c>
-      <c r="R3">
-        <v>6</v>
-      </c>
-      <c r="S3">
-        <v>6</v>
-      </c>
-      <c r="T3">
-        <f t="shared" ref="T3" si="0">R3+P3</f>
-        <v>6.5</v>
-      </c>
-      <c r="U3">
-        <f t="shared" ref="U3" si="1">S3+Q3</f>
-        <v>6.5</v>
-      </c>
       <c r="V3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>118</v>
@@ -3135,7 +3109,7 @@
         <v>118</v>
       </c>
       <c r="F4">
-        <v>500</v>
+        <v>250</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -3146,11 +3120,8 @@
       <c r="J4">
         <v>3</v>
       </c>
-      <c r="T4">
-        <v>6</v>
-      </c>
-      <c r="U4">
-        <v>6</v>
+      <c r="M4">
+        <v>10</v>
       </c>
       <c r="V4" t="s">
         <v>121</v>
@@ -3158,54 +3129,81 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F5">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="I5">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="J5">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>1100</v>
       </c>
       <c r="M5">
         <v>10</v>
       </c>
+      <c r="N5">
+        <v>600</v>
+      </c>
+      <c r="O5">
+        <v>600</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5">
+        <v>0.5</v>
+      </c>
+      <c r="R5">
+        <v>6</v>
+      </c>
+      <c r="S5">
+        <v>6</v>
+      </c>
+      <c r="T5">
+        <v>6.5</v>
+      </c>
+      <c r="U5">
+        <v>6.5</v>
+      </c>
       <c r="V5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
         <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F6">
         <v>500</v>
@@ -3214,22 +3212,22 @@
         <v>2</v>
       </c>
       <c r="I6">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L6">
-        <v>2000</v>
+        <v>1100</v>
       </c>
       <c r="M6">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="N6">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="O6">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -3244,11 +3242,9 @@
         <v>6</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:U6" si="2">R6+P6</f>
         <v>6.5</v>
       </c>
       <c r="U6">
-        <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
       <c r="V6" t="s">
@@ -3257,13 +3253,13 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>118</v>
@@ -3272,27 +3268,208 @@
         <v>118</v>
       </c>
       <c r="F7">
-        <v>500</v>
+        <v>300</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>1000</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <v>1100</v>
+      </c>
+      <c r="M7">
+        <v>15</v>
+      </c>
+      <c r="N7">
+        <v>600</v>
+      </c>
+      <c r="O7">
+        <v>600</v>
+      </c>
+      <c r="P7">
+        <v>0.5</v>
+      </c>
+      <c r="Q7">
+        <v>0.5</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>3.5</v>
+      </c>
+      <c r="U7">
+        <v>3.5</v>
+      </c>
+      <c r="V7" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E8" t="s">
         <v>124</v>
       </c>
       <c r="F8">
         <v>500</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>1500</v>
+      </c>
+      <c r="M8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>600</v>
+      </c>
+      <c r="O8">
+        <v>600</v>
+      </c>
+      <c r="P8">
+        <v>0.5</v>
+      </c>
+      <c r="Q8">
+        <v>0.5</v>
+      </c>
+      <c r="R8">
+        <v>6</v>
+      </c>
+      <c r="S8">
+        <v>6</v>
+      </c>
+      <c r="T8">
+        <v>6.5</v>
+      </c>
+      <c r="U8">
+        <v>6.5</v>
+      </c>
+      <c r="V8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9">
+        <v>500</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1000</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>10</v>
+      </c>
+      <c r="V9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>124</v>
+      </c>
+      <c r="F10">
+        <v>500</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>1000</v>
+      </c>
+      <c r="J10">
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <v>1500</v>
+      </c>
+      <c r="M10">
+        <v>10</v>
+      </c>
+      <c r="N10">
+        <v>600</v>
+      </c>
+      <c r="O10">
+        <v>600</v>
+      </c>
+      <c r="P10">
+        <v>0.5</v>
+      </c>
+      <c r="Q10">
+        <v>0.5</v>
+      </c>
+      <c r="R10">
+        <v>6</v>
+      </c>
+      <c r="S10">
+        <v>6</v>
+      </c>
+      <c r="T10">
+        <v>6.5</v>
+      </c>
+      <c r="U10">
+        <v>6.5</v>
+      </c>
+      <c r="V10" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more scenarios including calendar view.
Also fixed bugs in calendar view.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03951AE6-2D00-6C46-BDB2-1B7DA70AFAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C09C172-C1E3-3C43-A627-A267DFB45D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="126">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -695,6 +695,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,15 +741,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,15 +754,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1098,105 +1098,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1243,16 +1243,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1753,11 +1753,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1773,6 +1768,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2932,11 +2932,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V10"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3321,49 +3321,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F8">
         <v>500</v>
       </c>
-      <c r="G8">
-        <v>2</v>
+      <c r="H8" s="1">
+        <v>44593</v>
       </c>
       <c r="I8">
         <v>1000</v>
       </c>
-      <c r="J8">
-        <v>10</v>
-      </c>
-      <c r="L8">
-        <v>1500</v>
-      </c>
-      <c r="M8">
-        <v>10</v>
+      <c r="K8" s="1">
+        <v>44614</v>
       </c>
       <c r="N8">
         <v>600</v>
       </c>
       <c r="O8">
         <v>600</v>
-      </c>
-      <c r="P8">
-        <v>0.5</v>
-      </c>
-      <c r="Q8">
-        <v>0.5</v>
-      </c>
-      <c r="R8">
-        <v>6</v>
-      </c>
-      <c r="S8">
-        <v>6</v>
       </c>
       <c r="T8">
         <v>6.5</v>
@@ -3383,10 +3365,10 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
         <v>124</v>
@@ -3401,24 +3383,51 @@
         <v>1000</v>
       </c>
       <c r="J9">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <v>1500</v>
       </c>
       <c r="M9">
         <v>10</v>
       </c>
+      <c r="N9">
+        <v>600</v>
+      </c>
+      <c r="O9">
+        <v>600</v>
+      </c>
+      <c r="P9">
+        <v>0.5</v>
+      </c>
+      <c r="Q9">
+        <v>0.5</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>6</v>
+      </c>
+      <c r="T9">
+        <v>6.5</v>
+      </c>
+      <c r="U9">
+        <v>6.5</v>
+      </c>
       <c r="V9" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
         <v>117</v>
@@ -3436,39 +3445,74 @@
         <v>1000</v>
       </c>
       <c r="J10">
-        <v>10</v>
-      </c>
-      <c r="L10">
-        <v>1500</v>
+        <v>3</v>
       </c>
       <c r="M10">
         <v>10</v>
       </c>
-      <c r="N10">
-        <v>600</v>
-      </c>
-      <c r="O10">
-        <v>600</v>
-      </c>
-      <c r="P10">
+      <c r="V10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11">
+        <v>500</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <v>1000</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>1500</v>
+      </c>
+      <c r="M11">
+        <v>10</v>
+      </c>
+      <c r="N11">
+        <v>600</v>
+      </c>
+      <c r="O11">
+        <v>600</v>
+      </c>
+      <c r="P11">
         <v>0.5</v>
       </c>
-      <c r="Q10">
+      <c r="Q11">
         <v>0.5</v>
       </c>
-      <c r="R10">
+      <c r="R11">
         <v>6</v>
       </c>
-      <c r="S10">
+      <c r="S11">
         <v>6</v>
       </c>
-      <c r="T10">
+      <c r="T11">
         <v>6.5</v>
       </c>
-      <c r="U10">
+      <c r="U11">
         <v>6.5</v>
       </c>
-      <c r="V10" t="s">
+      <c r="V11" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3483,7 +3527,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Got actual dimensions working!
Also centered visualizations in screen and removed flex layout since it wasn't needed.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C09C172-C1E3-3C43-A627-A267DFB45D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9A7642-74E7-4E4C-B4DE-A2814402A3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -2934,9 +2934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3162,10 +3162,10 @@
         <v>10</v>
       </c>
       <c r="N5">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O5">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="P5">
         <v>0.5</v>
@@ -3174,16 +3174,16 @@
         <v>0.5</v>
       </c>
       <c r="R5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T5">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="U5">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V5" t="s">
         <v>121</v>
@@ -3224,10 +3224,10 @@
         <v>15</v>
       </c>
       <c r="N6">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O6">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="P6">
         <v>0.5</v>
@@ -3236,16 +3236,16 @@
         <v>0.5</v>
       </c>
       <c r="R6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T6">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="U6">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V6" t="s">
         <v>121</v>
@@ -3286,10 +3286,10 @@
         <v>15</v>
       </c>
       <c r="N7">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O7">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="P7">
         <v>0.5</v>
@@ -3298,16 +3298,16 @@
         <v>0.5</v>
       </c>
       <c r="R7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T7">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="U7">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="V7" t="s">
         <v>121</v>
@@ -3342,16 +3342,16 @@
         <v>44614</v>
       </c>
       <c r="N8">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O8">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="T8">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="U8">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V8" t="s">
         <v>121</v>
@@ -3392,10 +3392,10 @@
         <v>10</v>
       </c>
       <c r="N9">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O9">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="P9">
         <v>0.5</v>
@@ -3404,16 +3404,16 @@
         <v>0.5</v>
       </c>
       <c r="R9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T9">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="U9">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V9" t="s">
         <v>121</v>
@@ -3489,10 +3489,10 @@
         <v>10</v>
       </c>
       <c r="N11">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="O11">
-        <v>600</v>
+        <v>100</v>
       </c>
       <c r="P11">
         <v>0.5</v>
@@ -3501,16 +3501,16 @@
         <v>0.5</v>
       </c>
       <c r="R11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S11">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T11">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="U11">
-        <v>6.5</v>
+        <v>8.5</v>
       </c>
       <c r="V11" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Checkin before trying to make table cells square
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9A7642-74E7-4E4C-B4DE-A2814402A3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298852F8-03C0-3E40-BD31-7B6A3A8E3E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -695,24 +695,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,6 +723,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,6 +745,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1098,105 +1098,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="39" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="49"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="55" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="S3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="50"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1243,16 +1243,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="54"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1753,6 +1753,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1768,11 +1773,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2934,9 +2934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q7" sqref="Q7"/>
+      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3348,10 +3348,10 @@
         <v>100</v>
       </c>
       <c r="T8">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="U8">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="V8" t="s">
         <v>121</v>
@@ -3420,7 +3420,7 @@
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="8">
+      <c r="A10">
         <v>5</v>
       </c>
       <c r="B10">

</xml_diff>

<commit_message>
Have bar drawing.  Need to fix alignment.
Bar is drawing.   I need to fix the alignment.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298852F8-03C0-3E40-BD31-7B6A3A8E3E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5924ABB0-8B8D-9748-A56C-CD42F20FE35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -695,6 +695,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -723,15 +741,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -745,15 +754,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1098,105 +1098,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1243,16 +1243,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1753,11 +1753,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1773,6 +1768,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2936,7 +2936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2944,6 +2944,7 @@
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" customWidth="1"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
     <col min="15" max="15" width="24.5" customWidth="1"/>
     <col min="16" max="16" width="19.1640625" customWidth="1"/>
@@ -3340,6 +3341,9 @@
       </c>
       <c r="K8" s="1">
         <v>44614</v>
+      </c>
+      <c r="L8">
+        <v>1100</v>
       </c>
       <c r="N8">
         <v>100</v>

</xml_diff>

<commit_message>
Clicking on bars works.
Added event handlers for clicking on bars.
Refactored code for cell creation to a method.
Moved styling from style sheet to code as inline styling.
Added 2 more questions for calendar without interactoin.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5924ABB0-8B8D-9748-A56C-CD42F20FE35F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B0E69-7167-D34F-A60F-AD84B82B382F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="126">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -2932,11 +2932,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V11"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3331,13 +3331,13 @@
         <v>118</v>
       </c>
       <c r="F8">
-        <v>500</v>
+        <v>300</v>
       </c>
       <c r="H8" s="1">
         <v>44593</v>
       </c>
       <c r="I8">
-        <v>1000</v>
+        <v>700</v>
       </c>
       <c r="K8" s="1">
         <v>44614</v>
@@ -3363,37 +3363,34 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F9">
         <v>500</v>
       </c>
-      <c r="G9">
-        <v>2</v>
+      <c r="H9" s="1">
+        <v>44593</v>
       </c>
       <c r="I9">
-        <v>1000</v>
-      </c>
-      <c r="J9">
-        <v>10</v>
+        <v>800</v>
+      </c>
+      <c r="K9" s="1">
+        <v>44617</v>
       </c>
       <c r="L9">
-        <v>1500</v>
-      </c>
-      <c r="M9">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="N9">
         <v>100</v>
@@ -3401,23 +3398,11 @@
       <c r="O9">
         <v>100</v>
       </c>
-      <c r="P9">
-        <v>0.5</v>
-      </c>
-      <c r="Q9">
-        <v>0.5</v>
-      </c>
-      <c r="R9">
+      <c r="T9">
         <v>8</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>8</v>
-      </c>
-      <c r="T9">
-        <v>8.5</v>
-      </c>
-      <c r="U9">
-        <v>8.5</v>
       </c>
       <c r="V9" t="s">
         <v>121</v>
@@ -3425,34 +3410,46 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E10" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F10">
-        <v>500</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
+        <v>300</v>
+      </c>
+      <c r="H10" s="1">
+        <v>44593</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="M10">
-        <v>10</v>
+      <c r="K10" s="1">
+        <v>44620</v>
+      </c>
+      <c r="L10">
+        <v>1100</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="T10">
+        <v>8</v>
+      </c>
+      <c r="U10">
+        <v>8</v>
       </c>
       <c r="V10" t="s">
         <v>121</v>
@@ -3460,7 +3457,7 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3469,7 +3466,7 @@
         <v>104</v>
       </c>
       <c r="D11" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E11" t="s">
         <v>124</v>
@@ -3517,6 +3514,197 @@
         <v>8.5</v>
       </c>
       <c r="V11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12">
+        <v>500</v>
+      </c>
+      <c r="H12" s="1">
+        <v>44593</v>
+      </c>
+      <c r="I12">
+        <v>1000</v>
+      </c>
+      <c r="K12" s="1">
+        <v>44614</v>
+      </c>
+      <c r="L12">
+        <v>1100</v>
+      </c>
+      <c r="N12">
+        <v>100</v>
+      </c>
+      <c r="O12">
+        <v>100</v>
+      </c>
+      <c r="T12">
+        <v>8</v>
+      </c>
+      <c r="U12">
+        <v>8</v>
+      </c>
+      <c r="V12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F13">
+        <v>500</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1000</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>10</v>
+      </c>
+      <c r="V13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14">
+        <v>500</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1000</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="L14">
+        <v>1500</v>
+      </c>
+      <c r="M14">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>100</v>
+      </c>
+      <c r="O14">
+        <v>100</v>
+      </c>
+      <c r="P14">
+        <v>0.5</v>
+      </c>
+      <c r="Q14">
+        <v>0.5</v>
+      </c>
+      <c r="R14">
+        <v>8</v>
+      </c>
+      <c r="S14">
+        <v>8</v>
+      </c>
+      <c r="T14">
+        <v>8.5</v>
+      </c>
+      <c r="U14">
+        <v>8.5</v>
+      </c>
+      <c r="V14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
+      </c>
+      <c r="F15">
+        <v>500</v>
+      </c>
+      <c r="H15" s="1">
+        <v>44593</v>
+      </c>
+      <c r="I15">
+        <v>1000</v>
+      </c>
+      <c r="K15" s="1">
+        <v>44614</v>
+      </c>
+      <c r="L15">
+        <v>1100</v>
+      </c>
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="O15">
+        <v>100</v>
+      </c>
+      <c r="T15">
+        <v>8</v>
+      </c>
+      <c r="U15">
+        <v>8</v>
+      </c>
+      <c r="V15" t="s">
         <v>121</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating the calendar view works with data change.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4B0E69-7167-D34F-A60F-AD84B82B382F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42C723-A09B-7A4E-9DCE-D5E2C6436791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -695,24 +695,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,6 +723,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,6 +745,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1098,105 +1098,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="39" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="49"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="55" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="S3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="50"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1243,16 +1243,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="54"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1753,6 +1753,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1768,11 +1773,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2936,7 +2936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3381,13 +3381,13 @@
         <v>500</v>
       </c>
       <c r="H9" s="1">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I9">
         <v>800</v>
       </c>
       <c r="K9" s="1">
-        <v>44617</v>
+        <v>44632</v>
       </c>
       <c r="L9">
         <v>1100</v>
@@ -3428,13 +3428,13 @@
         <v>300</v>
       </c>
       <c r="H10" s="1">
-        <v>44593</v>
+        <v>44652</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
       <c r="K10" s="1">
-        <v>44620</v>
+        <v>44666</v>
       </c>
       <c r="L10">
         <v>1100</v>

</xml_diff>

<commit_message>
Refactored instructions to use case statement.
Tried getting worded form to be restricted to since in inches like bar and calendar.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42C723-A09B-7A4E-9DCE-D5E2C6436791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A582F45C-D7CE-074B-A2AE-5E72D28CA510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -2936,7 +2936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3054,6 +3054,12 @@
       <c r="M2">
         <v>10</v>
       </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>4</v>
+      </c>
       <c r="V2" t="s">
         <v>121</v>
       </c>
@@ -3089,6 +3095,12 @@
       <c r="M3">
         <v>10</v>
       </c>
+      <c r="T3">
+        <v>8</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
       <c r="V3" t="s">
         <v>121</v>
       </c>
@@ -3123,6 +3135,12 @@
       </c>
       <c r="M4">
         <v>10</v>
+      </c>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>8</v>
       </c>
       <c r="V4" t="s">
         <v>121</v>
@@ -3594,6 +3612,12 @@
       </c>
       <c r="M13">
         <v>10</v>
+      </c>
+      <c r="T13">
+        <v>8</v>
+      </c>
+      <c r="U13">
+        <v>8</v>
       </c>
       <c r="V13" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
Added more test links.
Refactored instructions into switch statements.
Added more test links and all features fetched with more dynamic code to make adding additional links a cut and paste.  Couldn't figure out how to use jsx in a loop or we could have gotten rid of the need to maintain the test link page.
Have the comments out of the treatment file driving the test link page text.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A582F45C-D7CE-074B-A2AE-5E72D28CA510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86BBB4F-964B-FD42-B847-871BA33DD309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="2560" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -447,6 +447,42 @@
   </si>
   <si>
     <t>drag</t>
+  </si>
+  <si>
+    <t>Barchart MEL question with no interaction.</t>
+  </si>
+  <si>
+    <t>Worded MEL question with no interaction and Read 2001 example values.</t>
+  </si>
+  <si>
+    <t>Barchart MEL question with drag interaction.</t>
+  </si>
+  <si>
+    <t>Word MEL question with titration interaction.</t>
+  </si>
+  <si>
+    <t>Barchat MEL question with titration interaction.</t>
+  </si>
+  <si>
+    <t>calendarWord</t>
+  </si>
+  <si>
+    <t>calendarBar</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and titration interaction.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and no interaction.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with word and titration interaction.</t>
+  </si>
+  <si>
+    <t>calendarDrag</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and drag interaction.</t>
   </si>
 </sst>
 </file>
@@ -2932,11 +2968,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V15"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3061,7 +3097,7 @@
         <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -3102,7 +3138,7 @@
         <v>8</v>
       </c>
       <c r="V3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -3143,7 +3179,7 @@
         <v>8</v>
       </c>
       <c r="V4" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -3205,7 +3241,7 @@
         <v>8.5</v>
       </c>
       <c r="V5" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -3267,7 +3303,7 @@
         <v>8.5</v>
       </c>
       <c r="V6" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -3329,7 +3365,7 @@
         <v>4.5</v>
       </c>
       <c r="V7" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -3340,7 +3376,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="D8" t="s">
         <v>118</v>
@@ -3376,7 +3412,7 @@
         <v>8</v>
       </c>
       <c r="V8" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -3387,7 +3423,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
         <v>118</v>
@@ -3423,7 +3459,7 @@
         <v>8</v>
       </c>
       <c r="V9" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -3434,7 +3470,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
@@ -3470,7 +3506,7 @@
         <v>8</v>
       </c>
       <c r="V10" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -3532,7 +3568,7 @@
         <v>8.5</v>
       </c>
       <c r="V11" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -3620,7 +3656,7 @@
         <v>8</v>
       </c>
       <c r="V13" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -3682,7 +3718,7 @@
         <v>8.5</v>
       </c>
       <c r="V14" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -3693,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="D15" t="s">
         <v>117</v>
@@ -3729,7 +3765,101 @@
         <v>8</v>
       </c>
       <c r="V15" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16">
+        <v>500</v>
+      </c>
+      <c r="H16" s="1">
+        <v>44593</v>
+      </c>
+      <c r="I16">
+        <v>1000</v>
+      </c>
+      <c r="K16" s="1">
+        <v>44614</v>
+      </c>
+      <c r="L16">
+        <v>1100</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+      <c r="O16">
+        <v>100</v>
+      </c>
+      <c r="T16">
+        <v>8</v>
+      </c>
+      <c r="U16">
+        <v>8</v>
+      </c>
+      <c r="V16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17">
+        <v>500</v>
+      </c>
+      <c r="H17" s="1">
+        <v>44593</v>
+      </c>
+      <c r="I17">
+        <v>1000</v>
+      </c>
+      <c r="K17" s="1">
+        <v>44614</v>
+      </c>
+      <c r="L17">
+        <v>1100</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+      <c r="O17">
+        <v>100</v>
+      </c>
+      <c r="T17">
+        <v>8</v>
+      </c>
+      <c r="U17">
+        <v>8</v>
+      </c>
+      <c r="V17" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed drag interaction on calendar bar view.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86BBB4F-964B-FD42-B847-871BA33DD309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D7618-4980-BA4E-B83A-66D7A92A0A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="137">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -477,9 +477,6 @@
   </si>
   <si>
     <t>Calendar MEL question with word and titration interaction.</t>
-  </si>
-  <si>
-    <t>calendarDrag</t>
   </si>
   <si>
     <t>Calendar MEL question with barchart and drag interaction.</t>
@@ -731,6 +728,24 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -759,15 +774,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -781,15 +787,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1134,105 +1131,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="36" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="53"/>
+      <c r="N3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="53"/>
+      <c r="P3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="50"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1251,7 +1248,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1279,16 +1276,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1789,11 +1786,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1809,6 +1801,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2970,14 +2967,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V17" sqref="V17"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
@@ -3823,10 +3821,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D17" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E17" t="s">
         <v>124</v>
@@ -3859,7 +3857,7 @@
         <v>8</v>
       </c>
       <c r="V17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug with luxon date class.  Year table working.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D7618-4980-BA4E-B83A-66D7A92A0A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C5E63-AEB3-634C-8090-A1B6683559A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -470,25 +470,29 @@
     <t>calendarBar</t>
   </si>
   <si>
-    <t>Calendar MEL question with barchart and titration interaction.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with barchart and no interaction.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with word and titration interaction.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with barchart and drag interaction.</t>
+    <t>Calendar MEL question with barchart and drag interaction year calendar view.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and drag interaction month view.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with word and titration interaction month view.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and titration interaction month view.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with barchart and no interaction month view.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -673,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -728,24 +732,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -774,6 +760,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -788,6 +783,16 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,105 +1136,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="39" t="s">
+      <c r="C2" s="37"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="54" t="s">
+      <c r="I2" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54" t="s">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="39" t="s">
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="39" t="s">
+      <c r="W2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="36" t="s">
+      <c r="X2" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="36" t="s">
+      <c r="Y2" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="36" t="s">
+      <c r="Z2" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="36" t="s">
+      <c r="AA2" s="53" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="49"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="55" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="53" t="s">
+      <c r="M3" s="50"/>
+      <c r="N3" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="53" t="s">
+      <c r="O3" s="50"/>
+      <c r="P3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="50"/>
+      <c r="R3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="51" t="s">
+      <c r="S3" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="51" t="s">
+      <c r="T3" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="50"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1248,7 +1253,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="41"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1276,16 +1281,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="52"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="V4" s="41"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="38"/>
-      <c r="Y4" s="38"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37"/>
+      <c r="R4" s="49"/>
+      <c r="S4" s="49"/>
+      <c r="T4" s="49"/>
+      <c r="U4" s="49"/>
+      <c r="V4" s="47"/>
+      <c r="W4" s="47"/>
+      <c r="X4" s="55"/>
+      <c r="Y4" s="55"/>
+      <c r="Z4" s="55"/>
+      <c r="AA4" s="54"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1786,6 +1791,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1801,11 +1811,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2965,11 +2970,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2978,7 +2983,9 @@
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11" style="56"/>
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
+    <col min="11" max="11" width="11" style="56"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
     <col min="15" max="15" width="24.5" customWidth="1"/>
     <col min="16" max="16" width="19.1640625" customWidth="1"/>
@@ -3011,7 +3018,7 @@
       <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="56" t="s">
         <v>89</v>
       </c>
       <c r="I1" t="s">
@@ -3020,7 +3027,7 @@
       <c r="J1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="56" t="s">
         <v>92</v>
       </c>
       <c r="L1" t="s">
@@ -3385,13 +3392,13 @@
       <c r="F8">
         <v>300</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="56">
         <v>44593</v>
       </c>
       <c r="I8">
         <v>700</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="56">
         <v>44614</v>
       </c>
       <c r="L8">
@@ -3410,7 +3417,7 @@
         <v>8</v>
       </c>
       <c r="V8" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -3432,13 +3439,13 @@
       <c r="F9">
         <v>500</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="56">
         <v>44621</v>
       </c>
       <c r="I9">
         <v>800</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="56">
         <v>44632</v>
       </c>
       <c r="L9">
@@ -3457,7 +3464,7 @@
         <v>8</v>
       </c>
       <c r="V9" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -3479,13 +3486,13 @@
       <c r="F10">
         <v>300</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="56">
         <v>44652</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="56">
         <v>44666</v>
       </c>
       <c r="L10">
@@ -3504,7 +3511,7 @@
         <v>8</v>
       </c>
       <c r="V10" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -3588,13 +3595,13 @@
       <c r="F12">
         <v>500</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="56">
         <v>44593</v>
       </c>
       <c r="I12">
         <v>1000</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="56">
         <v>44614</v>
       </c>
       <c r="L12">
@@ -3738,13 +3745,13 @@
       <c r="F15">
         <v>500</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="56">
         <v>44593</v>
       </c>
       <c r="I15">
         <v>1000</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="56">
         <v>44614</v>
       </c>
       <c r="L15">
@@ -3763,7 +3770,7 @@
         <v>8</v>
       </c>
       <c r="V15" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -3785,13 +3792,13 @@
       <c r="F16">
         <v>500</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="56">
         <v>44593</v>
       </c>
       <c r="I16">
         <v>1000</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="56">
         <v>44614</v>
       </c>
       <c r="L16">
@@ -3832,13 +3839,13 @@
       <c r="F17">
         <v>500</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="56">
         <v>44593</v>
       </c>
       <c r="I17">
         <v>1000</v>
       </c>
-      <c r="K17" s="1">
+      <c r="K17" s="56">
         <v>44614</v>
       </c>
       <c r="L17">
@@ -3857,7 +3864,54 @@
         <v>8</v>
       </c>
       <c r="V17" t="s">
-        <v>136</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18">
+        <v>500</v>
+      </c>
+      <c r="H18" s="56">
+        <v>44593</v>
+      </c>
+      <c r="I18">
+        <v>1000</v>
+      </c>
+      <c r="K18" s="56">
+        <v>44835</v>
+      </c>
+      <c r="L18">
+        <v>1100</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+      <c r="O18">
+        <v>100</v>
+      </c>
+      <c r="T18">
+        <v>8</v>
+      </c>
+      <c r="U18">
+        <v>8</v>
+      </c>
+      <c r="V18" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added treatments for calendar year view and fixed bugs.
Solved problem with calendar year view throwing exception when updating calendar year view.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245C5E63-AEB3-634C-8090-A1B6683559A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F017785-8999-584E-9AEE-22B137C78C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -492,7 +492,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -732,6 +732,25 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,15 +779,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -783,16 +793,6 @@
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,105 +1136,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="36" t="s">
+      <c r="A2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="45" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="45" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="53" t="s">
+      <c r="X2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="53" t="s">
+      <c r="Y2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="53" t="s">
+      <c r="Z2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="53" t="s">
+      <c r="AA2" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="43"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="52" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50" t="s">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="50"/>
-      <c r="N3" s="50" t="s">
+      <c r="M3" s="54"/>
+      <c r="N3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="50"/>
-      <c r="P3" s="50" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="50"/>
-      <c r="R3" s="48" t="s">
+      <c r="Q3" s="54"/>
+      <c r="R3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="46"/>
-      <c r="W3" s="46"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="44"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1281,16 +1281,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="49"/>
-      <c r="S4" s="49"/>
-      <c r="T4" s="49"/>
-      <c r="U4" s="49"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="54"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="38"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1791,11 +1791,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1811,6 +1806,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2972,9 +2972,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2983,9 +2983,9 @@
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="11" style="56"/>
+    <col min="8" max="8" width="11" style="36"/>
     <col min="9" max="9" width="19.1640625" customWidth="1"/>
-    <col min="11" max="11" width="11" style="56"/>
+    <col min="11" max="11" width="11" style="36"/>
     <col min="14" max="14" width="19.5" customWidth="1"/>
     <col min="15" max="15" width="24.5" customWidth="1"/>
     <col min="16" max="16" width="19.1640625" customWidth="1"/>
@@ -3018,7 +3018,7 @@
       <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="36" t="s">
         <v>89</v>
       </c>
       <c r="I1" t="s">
@@ -3027,7 +3027,7 @@
       <c r="J1" t="s">
         <v>91</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="36" t="s">
         <v>92</v>
       </c>
       <c r="L1" t="s">
@@ -3392,13 +3392,13 @@
       <c r="F8">
         <v>300</v>
       </c>
-      <c r="H8" s="56">
+      <c r="H8" s="36">
         <v>44593</v>
       </c>
       <c r="I8">
         <v>700</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="36">
         <v>44614</v>
       </c>
       <c r="L8">
@@ -3439,13 +3439,13 @@
       <c r="F9">
         <v>500</v>
       </c>
-      <c r="H9" s="56">
+      <c r="H9" s="36">
         <v>44621</v>
       </c>
       <c r="I9">
         <v>800</v>
       </c>
-      <c r="K9" s="56">
+      <c r="K9" s="36">
         <v>44632</v>
       </c>
       <c r="L9">
@@ -3486,13 +3486,13 @@
       <c r="F10">
         <v>300</v>
       </c>
-      <c r="H10" s="56">
+      <c r="H10" s="36">
         <v>44652</v>
       </c>
       <c r="I10">
         <v>1000</v>
       </c>
-      <c r="K10" s="56">
+      <c r="K10" s="36">
         <v>44666</v>
       </c>
       <c r="L10">
@@ -3595,13 +3595,13 @@
       <c r="F12">
         <v>500</v>
       </c>
-      <c r="H12" s="56">
+      <c r="H12" s="36">
         <v>44593</v>
       </c>
       <c r="I12">
         <v>1000</v>
       </c>
-      <c r="K12" s="56">
+      <c r="K12" s="36">
         <v>44614</v>
       </c>
       <c r="L12">
@@ -3745,13 +3745,13 @@
       <c r="F15">
         <v>500</v>
       </c>
-      <c r="H15" s="56">
+      <c r="H15" s="36">
         <v>44593</v>
       </c>
       <c r="I15">
         <v>1000</v>
       </c>
-      <c r="K15" s="56">
+      <c r="K15" s="36">
         <v>44614</v>
       </c>
       <c r="L15">
@@ -3792,13 +3792,13 @@
       <c r="F16">
         <v>500</v>
       </c>
-      <c r="H16" s="56">
+      <c r="H16" s="36">
         <v>44593</v>
       </c>
       <c r="I16">
         <v>1000</v>
       </c>
-      <c r="K16" s="56">
+      <c r="K16" s="36">
         <v>44614</v>
       </c>
       <c r="L16">
@@ -3839,13 +3839,13 @@
       <c r="F17">
         <v>500</v>
       </c>
-      <c r="H17" s="56">
+      <c r="H17" s="36">
         <v>44593</v>
       </c>
       <c r="I17">
         <v>1000</v>
       </c>
-      <c r="K17" s="56">
+      <c r="K17" s="36">
         <v>44614</v>
       </c>
       <c r="L17">
@@ -3886,13 +3886,13 @@
       <c r="F18">
         <v>500</v>
       </c>
-      <c r="H18" s="56">
+      <c r="H18" s="36">
         <v>44593</v>
       </c>
       <c r="I18">
         <v>1000</v>
       </c>
-      <c r="K18" s="56">
+      <c r="K18" s="36">
         <v>44835</v>
       </c>
       <c r="L18">
@@ -3905,7 +3905,7 @@
         <v>100</v>
       </c>
       <c r="T18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="U18">
         <v>8</v>

</xml_diff>

<commit_message>
Updating working, added treatments, code cleanup.
I have the calendar bar chart and work updating correctly.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F017785-8999-584E-9AEE-22B137C78C6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FBD62A-A75C-454D-BD34-68F4CA57332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="139">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t>Calendar MEL question with barchart and no interaction month view.</t>
+  </si>
+  <si>
+    <t>Calendar MEL question with word and no interaction month view.</t>
   </si>
 </sst>
 </file>
@@ -2970,11 +2973,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U18" sqref="U18"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3522,31 +3525,28 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F11">
-        <v>500</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
+        <v>300</v>
+      </c>
+      <c r="H11" s="36">
+        <v>44593</v>
       </c>
       <c r="I11">
-        <v>1000</v>
-      </c>
-      <c r="J11">
-        <v>10</v>
+        <v>700</v>
+      </c>
+      <c r="K11" s="36">
+        <v>44614</v>
       </c>
       <c r="L11">
-        <v>1500</v>
-      </c>
-      <c r="M11">
-        <v>10</v>
+        <v>1100</v>
       </c>
       <c r="N11">
         <v>100</v>
@@ -3554,55 +3554,43 @@
       <c r="O11">
         <v>100</v>
       </c>
-      <c r="P11">
-        <v>0.5</v>
-      </c>
-      <c r="Q11">
-        <v>0.5</v>
-      </c>
-      <c r="R11">
+      <c r="T11">
         <v>8</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>8</v>
       </c>
-      <c r="T11">
-        <v>8.5</v>
-      </c>
-      <c r="U11">
-        <v>8.5</v>
-      </c>
       <c r="V11" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F12">
         <v>500</v>
       </c>
       <c r="H12" s="36">
-        <v>44593</v>
+        <v>44621</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>800</v>
       </c>
       <c r="K12" s="36">
-        <v>44614</v>
+        <v>44632</v>
       </c>
       <c r="L12">
         <v>1100</v>
@@ -3620,39 +3608,45 @@
         <v>8</v>
       </c>
       <c r="V12" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="F13">
-        <v>500</v>
-      </c>
-      <c r="G13">
-        <v>2</v>
+        <v>300</v>
+      </c>
+      <c r="H13" s="36">
+        <v>44652</v>
       </c>
       <c r="I13">
         <v>1000</v>
       </c>
-      <c r="J13">
-        <v>3</v>
-      </c>
-      <c r="M13">
-        <v>10</v>
+      <c r="K13" s="36">
+        <v>44666</v>
+      </c>
+      <c r="L13">
+        <v>1100</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="O13">
+        <v>100</v>
       </c>
       <c r="T13">
         <v>8</v>
@@ -3661,12 +3655,12 @@
         <v>8</v>
       </c>
       <c r="V13" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3675,7 +3669,7 @@
         <v>104</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E14" t="s">
         <v>124</v>
@@ -3723,21 +3717,21 @@
         <v>8.5</v>
       </c>
       <c r="V14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D15" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
         <v>124</v>
@@ -3770,18 +3764,18 @@
         <v>8</v>
       </c>
       <c r="V15" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
         <v>117</v>
@@ -3792,23 +3786,17 @@
       <c r="F16">
         <v>500</v>
       </c>
-      <c r="H16" s="36">
-        <v>44593</v>
+      <c r="G16">
+        <v>2</v>
       </c>
       <c r="I16">
         <v>1000</v>
       </c>
-      <c r="K16" s="36">
-        <v>44614</v>
-      </c>
-      <c r="L16">
-        <v>1100</v>
-      </c>
-      <c r="N16">
-        <v>100</v>
-      </c>
-      <c r="O16">
-        <v>100</v>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
       </c>
       <c r="T16">
         <v>8</v>
@@ -3817,21 +3805,21 @@
         <v>8</v>
       </c>
       <c r="V16" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E17" t="s">
         <v>124</v>
@@ -3839,17 +3827,20 @@
       <c r="F17">
         <v>500</v>
       </c>
-      <c r="H17" s="36">
-        <v>44593</v>
+      <c r="G17">
+        <v>2</v>
       </c>
       <c r="I17">
         <v>1000</v>
       </c>
-      <c r="K17" s="36">
-        <v>44614</v>
+      <c r="J17">
+        <v>10</v>
       </c>
       <c r="L17">
-        <v>1100</v>
+        <v>1500</v>
+      </c>
+      <c r="M17">
+        <v>10</v>
       </c>
       <c r="N17">
         <v>100</v>
@@ -3857,25 +3848,37 @@
       <c r="O17">
         <v>100</v>
       </c>
+      <c r="P17">
+        <v>0.5</v>
+      </c>
+      <c r="Q17">
+        <v>0.5</v>
+      </c>
+      <c r="R17">
+        <v>8</v>
+      </c>
+      <c r="S17">
+        <v>8</v>
+      </c>
       <c r="T17">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="U17">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="V17" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
         <v>117</v>
@@ -3893,7 +3896,7 @@
         <v>1000</v>
       </c>
       <c r="K18" s="36">
-        <v>44835</v>
+        <v>44614</v>
       </c>
       <c r="L18">
         <v>1100</v>
@@ -3905,12 +3908,153 @@
         <v>100</v>
       </c>
       <c r="T18">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U18">
         <v>8</v>
       </c>
       <c r="V18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>131</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19">
+        <v>500</v>
+      </c>
+      <c r="H19" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I19">
+        <v>1000</v>
+      </c>
+      <c r="K19" s="36">
+        <v>44614</v>
+      </c>
+      <c r="L19">
+        <v>1100</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+      <c r="O19">
+        <v>100</v>
+      </c>
+      <c r="T19">
+        <v>8</v>
+      </c>
+      <c r="U19">
+        <v>8</v>
+      </c>
+      <c r="V19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F20">
+        <v>500</v>
+      </c>
+      <c r="H20" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I20">
+        <v>1000</v>
+      </c>
+      <c r="K20" s="36">
+        <v>44614</v>
+      </c>
+      <c r="L20">
+        <v>1100</v>
+      </c>
+      <c r="N20">
+        <v>100</v>
+      </c>
+      <c r="O20">
+        <v>100</v>
+      </c>
+      <c r="T20">
+        <v>8</v>
+      </c>
+      <c r="U20">
+        <v>8</v>
+      </c>
+      <c r="V20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21">
+        <v>500</v>
+      </c>
+      <c r="H21" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I21">
+        <v>1000</v>
+      </c>
+      <c r="K21" s="36">
+        <v>44835</v>
+      </c>
+      <c r="L21">
+        <v>1100</v>
+      </c>
+      <c r="N21">
+        <v>100</v>
+      </c>
+      <c r="O21">
+        <v>100</v>
+      </c>
+      <c r="T21">
+        <v>10</v>
+      </c>
+      <c r="U21">
+        <v>8</v>
+      </c>
+      <c r="V21" t="s">
         <v>133</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I have year calendar working!
Need to fix the size of the earlier/later amount text.
Refined comment in test treatments.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FBD62A-A75C-454D-BD34-68F4CA57332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C0592B-1D36-C041-AFFC-142F9A5BC05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="140">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -452,40 +452,43 @@
     <t>Barchart MEL question with no interaction.</t>
   </si>
   <si>
-    <t>Worded MEL question with no interaction and Read 2001 example values.</t>
-  </si>
-  <si>
-    <t>Barchart MEL question with drag interaction.</t>
-  </si>
-  <si>
-    <t>Word MEL question with titration interaction.</t>
-  </si>
-  <si>
-    <t>Barchat MEL question with titration interaction.</t>
-  </si>
-  <si>
     <t>calendarWord</t>
   </si>
   <si>
     <t>calendarBar</t>
   </si>
   <si>
-    <t>Calendar MEL question with barchart and drag interaction year calendar view.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with barchart and drag interaction month view.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with word and titration interaction month view.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with barchart and titration interaction month view.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with barchart and no interaction month view.</t>
-  </si>
-  <si>
-    <t>Calendar MEL question with word and no interaction month view.</t>
+    <t>Calendar year view with word and titration interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with barchart and drag interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with word and titration interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with barchart and titration interaction.</t>
+  </si>
+  <si>
+    <t>Barchat with titration interaction.</t>
+  </si>
+  <si>
+    <t>Word with titration interaction.</t>
+  </si>
+  <si>
+    <t>Barchart with drag interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with word and no interaction.</t>
+  </si>
+  <si>
+    <t>Calendar month view with barchart and no interaction.</t>
+  </si>
+  <si>
+    <t>Barchart with no interaction.</t>
+  </si>
+  <si>
+    <t>Worded with no interaction and Read 2001 example values.</t>
   </si>
 </sst>
 </file>
@@ -736,24 +739,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -782,6 +767,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -795,6 +789,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1139,105 +1142,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55" t="s">
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="40" t="s">
+      <c r="W2" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="X2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Y2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AA2" s="54" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="50"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="56" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="51"/>
+      <c r="N3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54" t="s">
+      <c r="O3" s="51"/>
+      <c r="P3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="52" t="s">
+      <c r="Q3" s="51"/>
+      <c r="R3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="51"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1256,7 +1259,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1284,16 +1287,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="38"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="55"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1794,6 +1797,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1809,11 +1817,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2975,9 +2978,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -3105,7 +3108,7 @@
         <v>4</v>
       </c>
       <c r="V2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -3146,7 +3149,7 @@
         <v>8</v>
       </c>
       <c r="V3" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -3187,7 +3190,7 @@
         <v>8</v>
       </c>
       <c r="V4" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -3311,7 +3314,7 @@
         <v>8.5</v>
       </c>
       <c r="V6" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -3373,7 +3376,7 @@
         <v>4.5</v>
       </c>
       <c r="V7" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -3384,7 +3387,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D8" t="s">
         <v>118</v>
@@ -3431,7 +3434,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D9" t="s">
         <v>118</v>
@@ -3478,7 +3481,7 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D10" t="s">
         <v>118</v>
@@ -3525,7 +3528,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
         <v>118</v>
@@ -3561,7 +3564,7 @@
         <v>8</v>
       </c>
       <c r="V11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -3572,7 +3575,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D12" t="s">
         <v>118</v>
@@ -3608,7 +3611,7 @@
         <v>8</v>
       </c>
       <c r="V12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -3619,7 +3622,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
         <v>118</v>
@@ -3655,7 +3658,7 @@
         <v>8</v>
       </c>
       <c r="V13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -3717,7 +3720,7 @@
         <v>8.5</v>
       </c>
       <c r="V14" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -3805,7 +3808,7 @@
         <v>8</v>
       </c>
       <c r="V16" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:22">
@@ -3867,7 +3870,7 @@
         <v>8.5</v>
       </c>
       <c r="V17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:22">
@@ -3878,7 +3881,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
         <v>117</v>
@@ -3914,7 +3917,7 @@
         <v>8</v>
       </c>
       <c r="V18" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:22">
@@ -3925,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
         <v>117</v>
@@ -3961,7 +3964,7 @@
         <v>8</v>
       </c>
       <c r="V19" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -3972,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
         <v>125</v>
@@ -4008,7 +4011,7 @@
         <v>8</v>
       </c>
       <c r="V20" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:22">
@@ -4019,7 +4022,7 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
         <v>117</v>
@@ -4055,7 +4058,7 @@
         <v>8</v>
       </c>
       <c r="V21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Year word and barchart working.
I need to fix the bar font size and barchart size for the smaller calendar square.
I added additional test cases.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C0592B-1D36-C041-AFFC-142F9A5BC05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65FDD75-87D4-B741-80D8-667E6D418A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="141">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -489,6 +489,9 @@
   </si>
   <si>
     <t>Worded with no interaction and Read 2001 example values.</t>
+  </si>
+  <si>
+    <t>Calendar year view with barchart and drag interaction.</t>
   </si>
 </sst>
 </file>
@@ -739,6 +742,24 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -767,15 +788,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -789,15 +801,6 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,105 +1145,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="38"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="46" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52" t="s">
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="46" t="s">
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="54" t="s">
+      <c r="W2" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="54" t="s">
+      <c r="Y2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="54" t="s">
+      <c r="Z2" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="54" t="s">
+      <c r="AA2" s="37" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="44"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="53" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51" t="s">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="51" t="s">
+      <c r="M3" s="54"/>
+      <c r="N3" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="51"/>
-      <c r="P3" s="51" t="s">
+      <c r="O3" s="54"/>
+      <c r="P3" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="49" t="s">
+      <c r="Q3" s="54"/>
+      <c r="R3" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="49" t="s">
+      <c r="T3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="49" t="s">
+      <c r="U3" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="55"/>
-      <c r="Z3" s="55"/>
-      <c r="AA3" s="55"/>
+      <c r="V3" s="41"/>
+      <c r="W3" s="41"/>
+      <c r="X3" s="38"/>
+      <c r="Y3" s="38"/>
+      <c r="Z3" s="38"/>
+      <c r="AA3" s="38"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="45"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1259,7 +1262,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="48"/>
+      <c r="H4" s="42"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1287,16 +1290,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="50"/>
-      <c r="S4" s="50"/>
-      <c r="T4" s="50"/>
-      <c r="U4" s="50"/>
-      <c r="V4" s="48"/>
-      <c r="W4" s="48"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="55"/>
+      <c r="R4" s="53"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="39"/>
+      <c r="Y4" s="39"/>
+      <c r="Z4" s="39"/>
+      <c r="AA4" s="38"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1797,11 +1800,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1817,6 +1815,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2976,11 +2979,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V21"/>
+  <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V5" sqref="V5"/>
+      <selection pane="bottomLeft" activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4059,6 +4062,53 @@
       </c>
       <c r="V21" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="A22">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22">
+        <v>500</v>
+      </c>
+      <c r="H22" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I22">
+        <v>1000</v>
+      </c>
+      <c r="K22" s="36">
+        <v>44835</v>
+      </c>
+      <c r="L22">
+        <v>1100</v>
+      </c>
+      <c r="N22">
+        <v>100</v>
+      </c>
+      <c r="O22">
+        <v>100</v>
+      </c>
+      <c r="T22">
+        <v>10</v>
+      </c>
+      <c r="U22">
+        <v>8</v>
+      </c>
+      <c r="V22" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug with may month showing.
Added more test scenarios.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C65FDD75-87D4-B741-80D8-667E6D418A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0FA6DD-12B5-414B-8F99-BE907B0189D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="142">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -492,6 +492,9 @@
   </si>
   <si>
     <t>Calendar year view with barchart and drag interaction.</t>
+  </si>
+  <si>
+    <t>Calendar year view with word and no interaction.</t>
   </si>
 </sst>
 </file>
@@ -742,24 +745,6 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -788,6 +773,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -801,6 +795,15 @@
     </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1145,105 +1148,105 @@
       </c>
     </row>
     <row r="2" spans="1:27">
-      <c r="A2" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="43" t="s">
+      <c r="A2" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="40" t="s">
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="55" t="s">
+      <c r="I2" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55" t="s">
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="40" t="s">
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="37" t="s">
+      <c r="W2" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="X2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="Y2" s="37" t="s">
+      <c r="Y2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="37" t="s">
+      <c r="Z2" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="AA2" s="37" t="s">
+      <c r="AA2" s="54" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:27">
-      <c r="A3" s="50"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="56" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="53" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54" t="s">
+      <c r="M3" s="51"/>
+      <c r="N3" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54" t="s">
+      <c r="O3" s="51"/>
+      <c r="P3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="52" t="s">
+      <c r="Q3" s="51"/>
+      <c r="R3" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="52" t="s">
+      <c r="S3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="52" t="s">
+      <c r="T3" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="52" t="s">
+      <c r="U3" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="41"/>
-      <c r="W3" s="41"/>
-      <c r="X3" s="38"/>
-      <c r="Y3" s="38"/>
-      <c r="Z3" s="38"/>
-      <c r="AA3" s="38"/>
+      <c r="V3" s="47"/>
+      <c r="W3" s="47"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="55"/>
+      <c r="Z3" s="55"/>
+      <c r="AA3" s="55"/>
     </row>
     <row r="4" spans="1:27" ht="60">
-      <c r="A4" s="51"/>
+      <c r="A4" s="45"/>
       <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
@@ -1262,7 +1265,7 @@
       <c r="G4" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="42"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="21" t="s">
         <v>26</v>
       </c>
@@ -1290,16 +1293,16 @@
       <c r="Q4" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="R4" s="53"/>
-      <c r="S4" s="53"/>
-      <c r="T4" s="53"/>
-      <c r="U4" s="53"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="42"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="38"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="50"/>
+      <c r="T4" s="50"/>
+      <c r="U4" s="50"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="56"/>
+      <c r="Y4" s="56"/>
+      <c r="Z4" s="56"/>
+      <c r="AA4" s="55"/>
     </row>
     <row r="5" spans="1:27" ht="30">
       <c r="A5" s="23">
@@ -1800,6 +1803,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="AA2:AA4"/>
+    <mergeCell ref="Z2:Z4"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="X2:X4"/>
     <mergeCell ref="B2:D3"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="V2:V4"/>
@@ -1815,11 +1823,6 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="H2:H4"/>
-    <mergeCell ref="AA2:AA4"/>
-    <mergeCell ref="Z2:Z4"/>
-    <mergeCell ref="Y2:Y4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="X2:X4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2979,11 +2982,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V22" sqref="V22"/>
+      <selection pane="bottomLeft" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4109,6 +4112,147 @@
       </c>
       <c r="V22" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23">
+        <v>14</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23">
+        <v>300</v>
+      </c>
+      <c r="H23" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I23">
+        <v>700</v>
+      </c>
+      <c r="K23" s="36">
+        <v>44703</v>
+      </c>
+      <c r="L23">
+        <v>1100</v>
+      </c>
+      <c r="N23">
+        <v>100</v>
+      </c>
+      <c r="O23">
+        <v>100</v>
+      </c>
+      <c r="T23">
+        <v>10</v>
+      </c>
+      <c r="U23">
+        <v>8</v>
+      </c>
+      <c r="V23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24">
+        <v>500</v>
+      </c>
+      <c r="H24" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I24">
+        <v>800</v>
+      </c>
+      <c r="K24" s="36">
+        <v>44724</v>
+      </c>
+      <c r="L24">
+        <v>1100</v>
+      </c>
+      <c r="N24">
+        <v>100</v>
+      </c>
+      <c r="O24">
+        <v>100</v>
+      </c>
+      <c r="T24">
+        <v>10</v>
+      </c>
+      <c r="U24">
+        <v>8</v>
+      </c>
+      <c r="V24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="A25">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25">
+        <v>300</v>
+      </c>
+      <c r="H25" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I25">
+        <v>1000</v>
+      </c>
+      <c r="K25" s="36">
+        <v>44757</v>
+      </c>
+      <c r="L25">
+        <v>1100</v>
+      </c>
+      <c r="N25">
+        <v>100</v>
+      </c>
+      <c r="O25">
+        <v>100</v>
+      </c>
+      <c r="T25">
+        <v>10</v>
+      </c>
+      <c r="U25">
+        <v>8</v>
+      </c>
+      <c r="V25" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new treatment for year calendar no interaction
Tried with two different approaches to get pop up amounts on hover over that I could style more.
</commit_message>
<xml_diff>
--- a/doc/MCL questions.xlsx
+++ b/doc/MCL questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/vizsurvey/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0FA6DD-12B5-414B-8F99-BE907B0189D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48F8932-6DB6-1D41-AC52-602BFBACFA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
+    <workbookView xWindow="1280" yWindow="540" windowWidth="35840" windowHeight="21060" activeTab="5" xr2:uid="{7432EDC4-6243-2543-BF06-3FCD944023A9}"/>
   </bookViews>
   <sheets>
     <sheet name="MCL" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="143">
   <si>
     <t>Proposed treatment parameters and estimated cost.</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>Calendar year view with word and no interaction.</t>
+  </si>
+  <si>
+    <t>Calendar year view with bar and no interaction.</t>
   </si>
 </sst>
 </file>
@@ -2982,11 +2985,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED366C34-5A3E-9A45-83C3-0286FA157D98}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V26" sqref="V26"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -4253,6 +4256,147 @@
       </c>
       <c r="V25" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="A26">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D26" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26">
+        <v>300</v>
+      </c>
+      <c r="H26" s="36">
+        <v>44593</v>
+      </c>
+      <c r="I26">
+        <v>700</v>
+      </c>
+      <c r="K26" s="36">
+        <v>44703</v>
+      </c>
+      <c r="L26">
+        <v>1100</v>
+      </c>
+      <c r="N26">
+        <v>100</v>
+      </c>
+      <c r="O26">
+        <v>100</v>
+      </c>
+      <c r="T26">
+        <v>10</v>
+      </c>
+      <c r="U26">
+        <v>8</v>
+      </c>
+      <c r="V26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="A27">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>128</v>
+      </c>
+      <c r="D27" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27">
+        <v>500</v>
+      </c>
+      <c r="H27" s="36">
+        <v>44621</v>
+      </c>
+      <c r="I27">
+        <v>800</v>
+      </c>
+      <c r="K27" s="36">
+        <v>44724</v>
+      </c>
+      <c r="L27">
+        <v>1100</v>
+      </c>
+      <c r="N27">
+        <v>100</v>
+      </c>
+      <c r="O27">
+        <v>100</v>
+      </c>
+      <c r="T27">
+        <v>10</v>
+      </c>
+      <c r="U27">
+        <v>8</v>
+      </c>
+      <c r="V27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D28" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28">
+        <v>300</v>
+      </c>
+      <c r="H28" s="36">
+        <v>44652</v>
+      </c>
+      <c r="I28">
+        <v>1000</v>
+      </c>
+      <c r="K28" s="36">
+        <v>44757</v>
+      </c>
+      <c r="L28">
+        <v>1100</v>
+      </c>
+      <c r="N28">
+        <v>100</v>
+      </c>
+      <c r="O28">
+        <v>100</v>
+      </c>
+      <c r="T28">
+        <v>10</v>
+      </c>
+      <c r="U28">
+        <v>8</v>
+      </c>
+      <c r="V28" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>